<commit_message>
ajout des FICHES et GANTT
</commit_message>
<xml_diff>
--- a/RAPPORT DE STAGE/Fiches Journalières.xlsx
+++ b/RAPPORT DE STAGE/Fiches Journalières.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t xml:space="preserve">26/06/2017 au 30/06/2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assignation</t>
   </si>
 </sst>
 </file>
@@ -434,7 +431,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -475,18 +472,14 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -497,30 +490,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -616,10 +585,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D65536"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -631,7 +600,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="39.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="47.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -645,7 +614,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="29.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
         <v>42849</v>
       </c>
@@ -659,7 +628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="29.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
         <v>42850</v>
       </c>
@@ -673,7 +642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="29.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -687,7 +656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="29.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -701,7 +670,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="29.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="n">
         <v>42858</v>
       </c>
@@ -715,7 +684,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="29.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="n">
         <v>42859</v>
       </c>
@@ -729,7 +698,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="29.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="n">
         <v>42860</v>
       </c>
@@ -743,7 +712,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="29.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
         <v>18</v>
       </c>
@@ -757,7 +726,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="29.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
         <v>19</v>
       </c>
@@ -771,146 +740,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="n">
-        <v>42881</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="n">
-        <v>42886</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="15" t="n">
-        <v>5</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="15" t="n">
-        <v>3</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="15" t="n">
-        <v>5</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="15" t="n">
-        <v>5</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -927,103 +757,176 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.66"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
+    <row r="1" customFormat="false" ht="48.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="16" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="18"/>
-    </row>
-    <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="18"/>
-    </row>
-    <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="18"/>
-    </row>
-    <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="18"/>
-    </row>
-    <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="18"/>
-    </row>
-    <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="18"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="20"/>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="20"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="26.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="26.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="n">
+        <v>42881</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="26.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="26.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="n">
+        <v>42886</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="26.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="26.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="14" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="26.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="26.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="26.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="14" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="14" t="n">
+        <v>5</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C9" type="list">
-      <formula1>"Anthony,Sophie,Anthony &amp; Sophie"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>